<commit_message>
update ls01 theory quiz xlsx
</commit_message>
<xml_diff>
--- a/quizzes/ls01_gg_intro/ls01_gg_intro_data_quiz/idar_ls01_gg_intro_data_quiz.xlsx
+++ b/quizzes/ls01_gg_intro/ls01_gg_intro_data_quiz/idar_ls01_gg_intro_data_quiz.xlsx
@@ -95,17 +95,18 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;script src="01_files/core-js-2.5.3/shim.min.js"&gt;&lt;/script&gt;
-&lt;script src="01_files/react-17.0.0/react.min.js"&gt;&lt;/script&gt;
-&lt;script src="01_files/react-17.0.0/react-dom.min.js"&gt;&lt;/script&gt;
-&lt;script src="01_files/reactwidget-1.0.0/react-tools.js"&gt;&lt;/script&gt;
-&lt;script src="01_files/htmlwidgets-1.5.4/htmlwidgets.js"&gt;&lt;/script&gt;
-&lt;script src="01_files/reactable-binding-0.3.0/reactable.js"&gt;&lt;/script&gt;
+    <t xml:space="preserve">
 &lt;p&gt;Welcome to your first data-based quiz on data visualization! For data-based quizzes, you will need to import data into R as you follow the questions.&lt;/p&gt;
 &lt;p&gt;Note that each time you retry a quiz, the dataset is slightly modified.&lt;/p&gt;
 &lt;div id="hiv-dataset" class="section level1"&gt;
 &lt;h1&gt;HIV dataset&lt;/h1&gt;
 &lt;p&gt;Here, you will analyze parts of a dataset documenting global HIV prevalence from 1990 to 2011.&lt;/p&gt;
+&lt;p&gt;Click &lt;a href="https://drive.google.com/file/d/1DjcpRAWXaWZECRpUZIKYR01c7wh7EBlG/view?usp=drivesdk" target="_blank"&gt;&lt;strong&gt;here&lt;/strong&gt;&lt;/a&gt; to view and download the data. Or import it directly into R with the code below:&lt;/p&gt;
+&lt;pre&gt;&lt;code&gt;if(!require(pacman)) install.packages(&amp;quot;pacman&amp;quot;)   
+pacman::p_load(rio)   
+hiv_prevalence &amp;lt;- import(&amp;quot;https://docs.google.com/uc?id=1DjcpRAWXaWZECRpUZIKYR01c7wh7EBlG&amp;amp;export=download&amp;quot;,
+ format = &amp;quot;csv&amp;quot;,
+ setclass = &amp;quot;tibble&amp;quot;)  &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;Here are the top 6 rows of &lt;code&gt;hiv_prevalence&lt;/code&gt; after import:&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;head(hiv_prevalence)&lt;/code&gt;&lt;/pre&gt;
 &lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 4
@@ -136,14 +137,14 @@
 ## &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;&lt;strong&gt;Complete the code below to create a scatter plot of HIV incidence over time.&lt;/strong&gt;&lt;/p&gt;
 &lt;p&gt;Hint: You plot should look like this:&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=1nAlPi0TqOg4ipQuYCdu0BTxzpP0AxGZm" width="480" /&gt;&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=1SAZ98XmvjVMufT4pmBI-NQS36Ej0iL-L" width="480" /&gt;&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;ggplot(data = {hiv_prevalence}, 
        {mapping} = aes({x} = year,
                        y = {total_cases})) {+}
   geom{_point}()&lt;/code&gt;&lt;/pre&gt;
 &lt;hr /&gt;
 &lt;p&gt;Make this plot and save it as an R object:
-&lt;img src="https://drive.google.com/uc?export=view&amp;id=1Xx9syeZEeVlj-XO2n0768bfSFoNHpjm7" width="672" /&gt;&lt;/p&gt;
+&lt;img src="https://drive.google.com/uc?export=view&amp;id=1xc85TX30oiQBEmia9Evou-tG8b9NBbPh" width="672" /&gt;&lt;/p&gt;
 &lt;p&gt;Put your plot object through the &lt;code&gt;ggplot_digest()&lt;/code&gt; function and enter the resulting character string here: {9fb1cf69b4fde79134ffb871ae01bf56}&lt;/p&gt;
 &lt;/div&gt;</t>
   </si>
@@ -160,6 +161,12 @@
 &lt;div id="hiv-dataset" class="section level1"&gt;
 &lt;h1&gt;HIV dataset&lt;/h1&gt;
 &lt;p&gt;Here, you will analyze parts of a dataset documenting global HIV prevalence from 1990 to 2011.&lt;/p&gt;
+&lt;p&gt;Click &lt;a href="https://drive.google.com/file/d/10UHloNs7wu1ES2aTJHsiC-iOBP615vUu/view?usp=drivesdk" target="_blank"&gt;&lt;strong&gt;here&lt;/strong&gt;&lt;/a&gt; to view and download the data. Or import it directly into R with the code below:&lt;/p&gt;
+&lt;pre&gt;&lt;code&gt;if(!require(pacman)) install.packages(&amp;quot;pacman&amp;quot;)   
+pacman::p_load(rio)   
+hiv_prevalence &amp;lt;- import(&amp;quot;https://docs.google.com/uc?id=10UHloNs7wu1ES2aTJHsiC-iOBP615vUu&amp;amp;export=download&amp;quot;,
+ format = &amp;quot;csv&amp;quot;,
+ setclass = &amp;quot;tibble&amp;quot;)  &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;Here are the top 6 rows of &lt;code&gt;hiv_prevalence&lt;/code&gt; after import:&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;head(hiv_prevalence)&lt;/code&gt;&lt;/pre&gt;
 &lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 4
@@ -190,14 +197,14 @@
 ## &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;&lt;strong&gt;Complete the code below to create a scatter plot of HIV incidence over time.&lt;/strong&gt;&lt;/p&gt;
 &lt;p&gt;Hint: You plot should look like this:&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=11adH9hO1tG9Jy1_1F5qVTh8IqwpzMtlN" width="480" /&gt;&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=1MJIjGZcM15tJv51ogPh3MlbYxFnpmKip" width="480" /&gt;&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;ggplot(data = {hiv_prevalence}, 
        {mapping} = aes({x} = year,
                        y = {total_cases})) {+}
   geom{_point}()&lt;/code&gt;&lt;/pre&gt;
 &lt;hr /&gt;
 &lt;p&gt;Make this plot and save it as an R object:
-&lt;img src="https://drive.google.com/uc?export=view&amp;id=1B96qCSocOaPmx7h_hvtJ8pHfQ9Xv5s7X" width="672" /&gt;&lt;/p&gt;
+&lt;img src="https://drive.google.com/uc?export=view&amp;id=1JsmOeM4rAwHylXTniph0axZOmjUHFr9y" width="672" /&gt;&lt;/p&gt;
 &lt;p&gt;Put your plot object through the &lt;code&gt;ggplot_digest()&lt;/code&gt; function and enter the resulting character string here: {865fce3a2bd569ad8ee8629e845e9b1e}&lt;/p&gt;
 &lt;/div&gt;</t>
   </si>
@@ -211,6 +218,12 @@
 &lt;div id="hiv-dataset" class="section level1"&gt;
 &lt;h1&gt;HIV dataset&lt;/h1&gt;
 &lt;p&gt;Here, you will analyze parts of a dataset documenting global HIV prevalence from 1990 to 2011.&lt;/p&gt;
+&lt;p&gt;Click &lt;a href="https://drive.google.com/file/d/1rIYcr4AuMCUmcQk8ED07tWhHx_WG0uNx/view?usp=drivesdk" target="_blank"&gt;&lt;strong&gt;here&lt;/strong&gt;&lt;/a&gt; to view and download the data. Or import it directly into R with the code below:&lt;/p&gt;
+&lt;pre&gt;&lt;code&gt;if(!require(pacman)) install.packages(&amp;quot;pacman&amp;quot;)   
+pacman::p_load(rio)   
+hiv_prevalence &amp;lt;- import(&amp;quot;https://docs.google.com/uc?id=1rIYcr4AuMCUmcQk8ED07tWhHx_WG0uNx&amp;amp;export=download&amp;quot;,
+ format = &amp;quot;csv&amp;quot;,
+ setclass = &amp;quot;tibble&amp;quot;)  &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;Here are the top 6 rows of &lt;code&gt;hiv_prevalence&lt;/code&gt; after import:&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;head(hiv_prevalence)&lt;/code&gt;&lt;/pre&gt;
 &lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 4
@@ -241,14 +254,14 @@
 ## &lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;&lt;strong&gt;Complete the code below to create a scatter plot of HIV incidence over time.&lt;/strong&gt;&lt;/p&gt;
 &lt;p&gt;Hint: You plot should look like this:&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=1czB7OmfMGN5_ogKwUejzpdAaJJhWXjmd" width="480" /&gt;&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;id=1WPJkQBDW6jGnSTS3zRw3GGfNvEeDaLEr" width="480" /&gt;&lt;/p&gt;
 &lt;pre class="r"&gt;&lt;code&gt;ggplot(data = {hiv_prevalence}, 
        {mapping} = aes({x} = year,
                        y = {total_cases})) {+}
   geom{_point}()&lt;/code&gt;&lt;/pre&gt;
 &lt;hr /&gt;
 &lt;p&gt;Make this plot and save it as an R object:
-&lt;img src="https://drive.google.com/uc?export=view&amp;id=1kwAsOMWjkPR0PaipYgHBBBl5bS6Vv_dd" width="672" /&gt;&lt;/p&gt;
+&lt;img src="https://drive.google.com/uc?export=view&amp;id=1hQNxU4hIFrNjhwk2DfKbsz7hpW6llXPZ" width="672" /&gt;&lt;/p&gt;
 &lt;p&gt;Put your plot object through the &lt;code&gt;ggplot_digest()&lt;/code&gt; function and enter the resulting character string here: {3b276234cebfd6a5d17fde35457e039b}&lt;/p&gt;
 &lt;/div&gt;</t>
   </si>

</xml_diff>